<commit_message>
Script 3, UI, & Second Ability
I got Unity Events working, formatted UI to keep the player informed about their movement and the Color Controller that's changing it, and gave the player the ability to shoot with damage a new Color Controller is changing to test multiple variables being changed at the same time.
</commit_message>
<xml_diff>
--- a/SIP Hours.xlsx
+++ b/SIP Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub Repositories\UAT-SIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E350AF-C3C0-4A6E-9F00-1603F406062D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BC835D-EE81-475B-8ECC-6C90094CACD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="150" windowWidth="16005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Month/Day/Year</t>
   </si>
@@ -102,6 +102,33 @@
   </si>
   <si>
     <t>5h2m</t>
+  </si>
+  <si>
+    <t>Script 3</t>
+  </si>
+  <si>
+    <t>12:22 to 1:22</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>1:25 to 2:43</t>
+  </si>
+  <si>
+    <t>1h18m</t>
+  </si>
+  <si>
+    <t>Second Ability</t>
+  </si>
+  <si>
+    <t>2:51 to 5:18</t>
+  </si>
+  <si>
+    <t>2h27m</t>
   </si>
 </sst>
 </file>
@@ -137,9 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +585,63 @@
         <v>17.02</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44918</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f>G6 + F7</f>
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>1.3</v>
+      </c>
+      <c r="G8">
+        <f>G7 + F8</f>
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G9">
+        <f>G8 + F9</f>
+        <v>21.77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>